<commit_message>
Adding updated capacity notebook and updated data
</commit_message>
<xml_diff>
--- a/ESG-Analysis/NewGeneratorCharacteristics_CapacityExpansion.xlsx
+++ b/ESG-Analysis/NewGeneratorCharacteristics_CapacityExpansion.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A\Box\EEP147\2024\ESG\Datahub\EEP-147-SP24\ESG-Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7066616B-420C-48AA-8276-1032D2E6843E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855E466A-100B-42BF-BC14-19BF709E1C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3675" yWindow="2880" windowWidth="37980" windowHeight="15120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NewGeneratorCharacteristics_TEM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -925,21 +925,20 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="479">
     <cellStyle name="20% - Accent1 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -1424,83 +1423,6 @@
   </cellStyles>
   <dxfs count="17">
     <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1793,6 +1715,49 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border outline="0">
         <top style="thin">
           <color auto="1"/>
@@ -1801,6 +1766,15 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
@@ -1808,18 +1782,43 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
         <right style="thin">
           <color auto="1"/>
         </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -1904,27 +1903,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D334D5BB-6454-4E7A-B94D-6E1BA140B3E2}" name="Table1" displayName="Table1" ref="A1:N6" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="15" tableBorderDxfId="16" totalsRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D334D5BB-6454-4E7A-B94D-6E1BA140B3E2}" name="Table1" displayName="Table1" ref="A1:N6" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15" tableBorderDxfId="14" totalsRowBorderDxfId="13">
   <autoFilter ref="A1:N6" xr:uid="{D334D5BB-6454-4E7A-B94D-6E1BA140B3E2}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{DAFF0583-07FF-4046-91D3-78751EB34550}" name="Plant_Type" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{2F8A7705-DA5F-4898-BFD2-755AA93C99C8}" name="Capacity_MW" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{DAFF0583-07FF-4046-91D3-78751EB34550}" name="Plant_Type" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{2F8A7705-DA5F-4898-BFD2-755AA93C99C8}" name="Capacity_MW" dataDxfId="11"/>
     <tableColumn id="3" xr3:uid="{F95B9ADE-2BB1-4DB7-B1E5-6787CD9E936B}" name="Heat_Rate_MMBtu_perMWH"/>
-    <tableColumn id="4" xr3:uid="{DD95C130-72D8-4AD4-86E2-C63C4AD73F26}" name="Fuel_Cost_USDperMMBtu" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{C2D29B68-7501-42C2-B1EC-464EA0FDA6A3}" name="Fuel_Cost_USDperMWH" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{16B6797C-36FB-4608-B306-AB3720040ED1}" name="Var_OandM_USDperMWH" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{480FD59F-FB65-4507-AC94-699F4B190BC1}" name="Var_Cost_USDperMWH" dataDxfId="10">
+    <tableColumn id="4" xr3:uid="{DD95C130-72D8-4AD4-86E2-C63C4AD73F26}" name="Fuel_Cost_USDperMMBtu" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{C2D29B68-7501-42C2-B1EC-464EA0FDA6A3}" name="Fuel_Cost_USDperMWH" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{16B6797C-36FB-4608-B306-AB3720040ED1}" name="Var_OandM_USDperMWH" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{480FD59F-FB65-4507-AC94-699F4B190BC1}" name="Var_Cost_USDperMWH" dataDxfId="7">
       <calculatedColumnFormula>E2+F2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{8B258EEB-42BC-468A-8D1F-01AF70FB62CB}" name="CO2_lbsperMMBtu" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{7CA35FF7-4C47-4C0A-85F9-CE45F13880F4}" name="Carbon_tonsperMWH" dataDxfId="8"/>
-    <tableColumn id="10" xr3:uid="{233231EC-80AB-42E1-85AC-E46B2A8276F0}" name="FixedCst_OandM_perkWperYear" dataDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{FCE7D5A4-EC5A-4430-A283-D2CC1B08D6F5}" name="FixedCst_OandM_perDay" dataDxfId="6">
+    <tableColumn id="8" xr3:uid="{8B258EEB-42BC-468A-8D1F-01AF70FB62CB}" name="CO2_lbsperMMBtu" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{7CA35FF7-4C47-4C0A-85F9-CE45F13880F4}" name="Carbon_tonsperMWH" dataDxfId="5">
+      <calculatedColumnFormula>H2*C2/2204.62</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{233231EC-80AB-42E1-85AC-E46B2A8276F0}" name="FixedCst_OandM_perkWperYear" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{FCE7D5A4-EC5A-4430-A283-D2CC1B08D6F5}" name="FixedCst_OandM_perDay" dataDxfId="3">
       <calculatedColumnFormula>J2*B2*1000/365</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{EACB9FD8-BE92-48BF-A37E-0FAA2F6D02DD}" name="CapEx_perkW" dataDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{3817C832-E320-4D87-8583-98D8B54DD472}" name="Construction_Financing_Cst_perkW" dataDxfId="4"/>
-    <tableColumn id="14" xr3:uid="{CDAB0F7A-2F31-4791-A115-821AE32555A6}" name="Capital_Expenditure_perMW" dataDxfId="3">
+    <tableColumn id="12" xr3:uid="{EACB9FD8-BE92-48BF-A37E-0FAA2F6D02DD}" name="CapEx_perkW" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{3817C832-E320-4D87-8583-98D8B54DD472}" name="Construction_Financing_Cst_perkW" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{CDAB0F7A-2F31-4791-A115-821AE32555A6}" name="Capital_Expenditure_perMW" dataDxfId="0">
       <calculatedColumnFormula>(L2+M2)*1000</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2253,109 +2254,108 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F5" sqref="F5"/>
+      <selection pane="topRight" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="26.28515625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="26.5703125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="24.28515625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="20" style="4" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="32.28515625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="31.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.42578125" style="4" customWidth="1"/>
-    <col min="13" max="13" width="34.5703125" style="4" customWidth="1"/>
-    <col min="14" max="14" width="29" style="4" customWidth="1"/>
-    <col min="15" max="16384" width="11.5703125" style="4"/>
+    <col min="1" max="1" width="14.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
+    <col min="6" max="6" width="26.5703125" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" customWidth="1"/>
+    <col min="8" max="8" width="20" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" customWidth="1"/>
+    <col min="10" max="10" width="32.28515625" customWidth="1"/>
+    <col min="11" max="11" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" customWidth="1"/>
+    <col min="13" max="13" width="34.5703125" customWidth="1"/>
+    <col min="14" max="14" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="5" customFormat="1">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:14" s="4" customFormat="1">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="1">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="C2" s="2">
         <v>8.49</v>
       </c>
       <c r="D2" s="2">
-        <v>2.41</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="E2" s="1">
         <f>D2*C2</f>
-        <v>20.460900000000002</v>
+        <v>21.6495</v>
       </c>
       <c r="F2" s="2">
         <v>9.3000000000000007</v>
       </c>
       <c r="G2" s="1">
         <f>E2+F2</f>
-        <v>29.760900000000003</v>
+        <v>30.9495</v>
       </c>
       <c r="H2" s="2">
         <v>202.3</v>
       </c>
       <c r="I2" s="1">
-        <f>H2*C2/2000</f>
-        <v>0.85876350000000001</v>
+        <f>H2*C2/2204.62</f>
+        <v>0.77905806896426599</v>
       </c>
       <c r="J2" s="2">
         <v>86.5</v>
       </c>
       <c r="K2" s="1">
         <f>J2*B2*1000/365</f>
-        <v>23698.630136986303</v>
+        <v>94794.520547945212</v>
       </c>
       <c r="L2" s="1">
         <v>4078.56</v>
@@ -2363,13 +2363,13 @@
       <c r="M2" s="2">
         <v>777.36</v>
       </c>
-      <c r="N2" s="7">
+      <c r="N2" s="6">
         <f>(L2+M2)*1000</f>
         <v>4855920</v>
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="1">
@@ -2379,25 +2379,25 @@
         <v>9.7170000000000005</v>
       </c>
       <c r="D3" s="3">
-        <v>6.45</v>
+        <v>3.03</v>
       </c>
       <c r="E3" s="1">
         <f>D3*C3</f>
-        <v>62.674650000000007</v>
+        <v>29.442509999999999</v>
       </c>
       <c r="F3" s="2">
         <v>6.94</v>
       </c>
       <c r="G3" s="1">
         <f>E3+F3</f>
-        <v>69.614650000000012</v>
+        <v>36.382509999999996</v>
       </c>
       <c r="H3" s="3">
         <v>119</v>
       </c>
       <c r="I3" s="1">
-        <f>H3*C3/2000</f>
-        <v>0.57816149999999999</v>
+        <f t="shared" ref="I3:I6" si="0">H3*C3/2204.62</f>
+        <v>0.52449991381734729</v>
       </c>
       <c r="J3" s="1">
         <v>26.1</v>
@@ -2412,24 +2412,27 @@
       <c r="M3" s="2">
         <v>138.41999999999999</v>
       </c>
-      <c r="N3" s="7">
+      <c r="N3" s="6">
         <f>(L3+M3)*1000</f>
         <v>1487240</v>
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="1">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="C4" s="3">
         <v>10.497</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="1">
+        <v>0.97</v>
+      </c>
       <c r="E4" s="1">
-        <v>10</v>
+        <f>D4*C4</f>
+        <v>10.182089999999999</v>
       </c>
       <c r="F4" s="1">
         <f>2.8</f>
@@ -2437,12 +2440,13 @@
       </c>
       <c r="G4" s="1">
         <f>E4+F4</f>
-        <v>12.8</v>
+        <v>12.982089999999999</v>
       </c>
       <c r="H4" s="1">
         <v>0</v>
       </c>
       <c r="I4" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J4" s="2">
@@ -2450,7 +2454,7 @@
       </c>
       <c r="K4" s="1">
         <f>J4*B4*1000/365</f>
-        <v>47945.205479452052</v>
+        <v>479452.05479452055</v>
       </c>
       <c r="L4" s="2">
         <v>7616.36</v>
@@ -2458,19 +2462,21 @@
       <c r="M4" s="2">
         <v>1766.36</v>
       </c>
-      <c r="N4" s="7">
+      <c r="N4" s="6">
         <f>(L4+M4)*1000</f>
         <v>9382720</v>
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="1">
         <v>100</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
       <c r="D5" s="1">
         <v>0</v>
       </c>
@@ -2488,6 +2494,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J5" s="1">
@@ -2503,52 +2510,55 @@
       <c r="M5" s="2">
         <v>94.23</v>
       </c>
-      <c r="N5" s="7">
+      <c r="N5" s="6">
         <f>(L5+M5)*1000</f>
         <v>1760020</v>
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="10">
         <v>100</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11">
+      <c r="C6" s="10">
         <v>0</v>
       </c>
-      <c r="E6" s="11">
+      <c r="D6" s="10">
         <v>0</v>
       </c>
-      <c r="F6" s="11">
+      <c r="E6" s="10">
         <v>0</v>
       </c>
-      <c r="G6" s="11">
+      <c r="F6" s="10">
+        <v>0</v>
+      </c>
+      <c r="G6" s="10">
         <f>E6+F6</f>
         <v>0</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="10">
         <v>0</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="10">
         <v>23.765603456360498</v>
       </c>
-      <c r="K6" s="11">
+      <c r="K6" s="10">
         <f>J6*B6*1000/365</f>
         <v>6511.1242346193158</v>
       </c>
-      <c r="L6" s="11">
+      <c r="L6" s="10">
         <v>1482.68</v>
       </c>
-      <c r="M6" s="11">
+      <c r="M6" s="10">
         <v>51.29</v>
       </c>
-      <c r="N6" s="12">
+      <c r="N6" s="11">
         <f>(L6+M6)*1000</f>
         <v>1533970</v>
       </c>

</xml_diff>